<commit_message>
Config changes and the permission matrix changes to include the role permissions for MQ, Tokenization, Data Gateway
</commit_message>
<xml_diff>
--- a/src/main/resources/files/custom_roles.xlsx
+++ b/src/main/resources/files/custom_roles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpaluri/Kishore/Development/MuleSoft/Studio-Workspaces/my-templates-ws/anypoint-access-management/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04683E18-54C6-BA41-A0EE-4DF431678ABF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64F6DE8-DBD1-CB48-965D-8AEA192BE625}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="matrix" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="64">
   <si>
     <t>Deploy API proxies</t>
   </si>
@@ -175,6 +175,48 @@
   </si>
   <si>
     <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>API Group Administrator</t>
+  </si>
+  <si>
+    <t>Manage Application Flows</t>
+  </si>
+  <si>
+    <t>MQ</t>
+  </si>
+  <si>
+    <t>Clear destinations</t>
+  </si>
+  <si>
+    <t>Manage clients</t>
+  </si>
+  <si>
+    <t>Manage destinations</t>
+  </si>
+  <si>
+    <t>View clients</t>
+  </si>
+  <si>
+    <t>View destinations</t>
+  </si>
+  <si>
+    <t>Tokenization</t>
+  </si>
+  <si>
+    <t>Manage Tokenization Formats</t>
+  </si>
+  <si>
+    <t>Manage Tokenization Services</t>
+  </si>
+  <si>
+    <t>Data Gateway Administrator</t>
+  </si>
+  <si>
+    <t>Data Gateway</t>
+  </si>
+  <si>
+    <t>Data Gateway Viewer</t>
   </si>
 </sst>
 </file>
@@ -550,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9D4BD7-9532-E647-A510-D27F49907965}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,11 +637,11 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -609,18 +651,14 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -629,10 +667,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>35</v>
@@ -640,9 +678,7 @@
       <c r="E4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -650,10 +686,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>35</v>
@@ -661,7 +697,9 @@
       <c r="E5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -669,7 +707,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>34</v>
@@ -680,9 +718,7 @@
       <c r="E6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -690,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>34</v>
@@ -711,10 +747,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>35</v>
@@ -725,16 +761,14 @@
       <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>35</v>
@@ -748,14 +782,16 @@
       <c r="F9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>35</v>
@@ -776,7 +812,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>35</v>
@@ -794,19 +830,23 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -814,11 +854,9 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
@@ -833,9 +871,11 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
@@ -850,16 +890,14 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -869,7 +907,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>34</v>
@@ -888,10 +926,10 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>35</v>
@@ -907,7 +945,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>35</v>
@@ -925,10 +963,12 @@
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>35</v>
       </c>
@@ -942,12 +982,10 @@
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>35</v>
       </c>
@@ -962,7 +1000,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>34</v>
@@ -981,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>34</v>
@@ -1000,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>34</v>
@@ -1019,7 +1057,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>34</v>
@@ -1038,10 +1076,10 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>35</v>
@@ -1049,19 +1087,15 @@
       <c r="E25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>35</v>
@@ -1084,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>35</v>
@@ -1104,93 +1138,99 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D31" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -1200,11 +1240,9 @@
         <v>43</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
         <v>35</v>
       </c>
@@ -1219,7 +1257,7 @@
         <v>43</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
@@ -1230,6 +1268,215 @@
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the anypoint monitoring roleIds and permissions
</commit_message>
<xml_diff>
--- a/src/main/resources/files/custom_roles.xlsx
+++ b/src/main/resources/files/custom_roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kpaluri/Kishore/Development/MuleSoft/Studio-Workspaces/my-templates-ws/anypoint-access-management/src/main/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64F6DE8-DBD1-CB48-965D-8AEA192BE625}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF845546-75A3-034C-B95A-A62F391C419C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="matrix" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="65">
   <si>
     <t>Deploy API proxies</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Anypoint Monitoring</t>
   </si>
   <si>
-    <t>Anypoint Monitoring User</t>
-  </si>
-  <si>
     <t>Visualizer</t>
   </si>
   <si>
@@ -217,6 +214,12 @@
   </si>
   <si>
     <t>Data Gateway Viewer</t>
+  </si>
+  <si>
+    <t>Monitoring Viewer</t>
+  </si>
+  <si>
+    <t>Monitoring Administrator</t>
   </si>
 </sst>
 </file>
@@ -592,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9D4BD7-9532-E647-A510-D27F49907965}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -626,7 +629,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>38</v>
@@ -637,7 +640,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
@@ -676,7 +679,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -695,7 +698,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>35</v>
@@ -716,7 +719,7 @@
         <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -735,7 +738,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>35</v>
@@ -756,7 +759,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>35</v>
@@ -777,7 +780,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>35</v>
@@ -800,7 +803,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>35</v>
@@ -821,7 +824,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>35</v>
@@ -842,7 +845,7 @@
         <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>35</v>
@@ -916,7 +919,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -935,7 +938,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -954,7 +957,7 @@
         <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -973,7 +976,7 @@
         <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -990,7 +993,7 @@
         <v>35</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1009,7 +1012,7 @@
         <v>35</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1028,7 +1031,7 @@
         <v>35</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1047,7 +1050,7 @@
         <v>35</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1066,7 +1069,7 @@
         <v>35</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1085,7 +1088,7 @@
         <v>35</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1104,7 +1107,7 @@
         <v>35</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>35</v>
@@ -1127,7 +1130,7 @@
         <v>35</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>35</v>
@@ -1150,7 +1153,7 @@
         <v>35</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>35</v>
@@ -1164,7 +1167,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>34</v>
@@ -1200,7 +1203,7 @@
         <v>39</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>33</v>
@@ -1220,12 +1223,14 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D32" s="2" t="s">
         <v>33</v>
       </c>
@@ -1237,100 +1242,98 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D36" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C38" s="2" t="s">
         <v>34</v>
       </c>
@@ -1338,17 +1341,17 @@
         <v>35</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>34</v>
@@ -1357,17 +1360,17 @@
         <v>35</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>34</v>
@@ -1376,19 +1379,17 @@
         <v>35</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>34</v>
@@ -1397,7 +1398,7 @@
         <v>35</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>34</v>
@@ -1406,44 +1407,46 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>34</v>
@@ -1452,31 +1455,50 @@
         <v>35</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G45" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>